<commit_message>
return to system pressure after outage was wrong date. sludge had wrong initial value (order of magnitude too high)
</commit_message>
<xml_diff>
--- a/FACModel/PLNGS_Power_Estimated (Pre 1996).xlsx
+++ b/FACModel/PLNGS_Power_Estimated (Pre 1996).xlsx
@@ -35506,7 +35506,7 @@
         <v>34802</v>
       </c>
       <c r="B4390">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4391" spans="1:2">
@@ -35514,7 +35514,7 @@
         <v>34803</v>
       </c>
       <c r="B4391">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4392" spans="1:2">
@@ -35522,7 +35522,7 @@
         <v>34804</v>
       </c>
       <c r="B4392">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4393" spans="1:2">
@@ -35530,7 +35530,7 @@
         <v>34805</v>
       </c>
       <c r="B4393">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4394" spans="1:2">
@@ -35538,7 +35538,7 @@
         <v>34806</v>
       </c>
       <c r="B4394">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4395" spans="1:2">
@@ -35546,7 +35546,7 @@
         <v>34807</v>
       </c>
       <c r="B4395">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4396" spans="1:2">
@@ -35554,7 +35554,7 @@
         <v>34808</v>
       </c>
       <c r="B4396">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4397" spans="1:2">
@@ -35562,7 +35562,7 @@
         <v>34809</v>
       </c>
       <c r="B4397">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4398" spans="1:2">
@@ -35570,7 +35570,7 @@
         <v>34810</v>
       </c>
       <c r="B4398">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4399" spans="1:2">
@@ -35578,7 +35578,7 @@
         <v>34811</v>
       </c>
       <c r="B4399">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4400" spans="1:2">
@@ -35586,7 +35586,7 @@
         <v>34812</v>
       </c>
       <c r="B4400">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4401" spans="1:2">
@@ -35594,7 +35594,7 @@
         <v>34813</v>
       </c>
       <c r="B4401">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4402" spans="1:2">
@@ -35602,7 +35602,7 @@
         <v>34814</v>
       </c>
       <c r="B4402">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4403" spans="1:2">
@@ -35610,7 +35610,7 @@
         <v>34815</v>
       </c>
       <c r="B4403">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4404" spans="1:2">
@@ -35618,7 +35618,7 @@
         <v>34816</v>
       </c>
       <c r="B4404">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4405" spans="1:2">
@@ -35626,7 +35626,7 @@
         <v>34817</v>
       </c>
       <c r="B4405">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4406" spans="1:2">
@@ -35634,7 +35634,7 @@
         <v>34818</v>
       </c>
       <c r="B4406">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4407" spans="1:2">
@@ -35642,7 +35642,7 @@
         <v>34819</v>
       </c>
       <c r="B4407">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4408" spans="1:2">
@@ -35650,7 +35650,7 @@
         <v>34820</v>
       </c>
       <c r="B4408">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4409" spans="1:2">
@@ -35658,7 +35658,7 @@
         <v>34821</v>
       </c>
       <c r="B4409">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4410" spans="1:2">
@@ -35666,7 +35666,7 @@
         <v>34822</v>
       </c>
       <c r="B4410">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4411" spans="1:2">
@@ -35674,7 +35674,7 @@
         <v>34823</v>
       </c>
       <c r="B4411">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4412" spans="1:2">
@@ -35682,7 +35682,7 @@
         <v>34824</v>
       </c>
       <c r="B4412">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4413" spans="1:2">
@@ -35690,7 +35690,7 @@
         <v>34825</v>
       </c>
       <c r="B4413">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4414" spans="1:2">
@@ -35698,7 +35698,7 @@
         <v>34826</v>
       </c>
       <c r="B4414">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4415" spans="1:2">
@@ -35706,7 +35706,7 @@
         <v>34827</v>
       </c>
       <c r="B4415">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4416" spans="1:2">
@@ -35714,7 +35714,7 @@
         <v>34828</v>
       </c>
       <c r="B4416">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4417" spans="1:2">
@@ -35722,7 +35722,7 @@
         <v>34829</v>
       </c>
       <c r="B4417">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4418" spans="1:2">
@@ -35730,7 +35730,7 @@
         <v>34830</v>
       </c>
       <c r="B4418">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4419" spans="1:2">
@@ -35738,7 +35738,7 @@
         <v>34831</v>
       </c>
       <c r="B4419">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4420" spans="1:2">

</xml_diff>